<commit_message>
update Nina's ands Sasha's chapters
</commit_message>
<xml_diff>
--- a/data/glosses.xlsx
+++ b/data/glosses.xlsx
@@ -153,7 +153,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="134">
   <si>
     <t xml:space="preserve">gloss</t>
   </si>
@@ -339,6 +339,30 @@
   </si>
   <si>
     <t xml:space="preserve">non-neuter pronominal suffix</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALL2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">allative</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EXST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">existential copula</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ORIENT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">orientational marker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">THITHER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">thither</t>
   </si>
   <si>
     <t xml:space="preserve">problem</t>
@@ -807,10 +831,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:C1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B31" activeCellId="0" sqref="B31"/>
+      <selection pane="topLeft" activeCell="B35" activeCellId="0" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1069,6 +1093,40 @@
         <v>61</v>
       </c>
     </row>
+    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
@@ -1091,7 +1149,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="57.75"/>
@@ -1104,16 +1162,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="F1" s="9"/>
       <c r="G1" s="9"/>
@@ -1139,165 +1197,165 @@
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="10" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="D2" s="12"/>
       <c r="E2" s="13" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="14" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="D3" s="16"/>
       <c r="E3" s="13" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="10" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="D4" s="12"/>
       <c r="E4" s="13" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="10" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="10" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="10" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="10" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="C9" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="D9" s="17" t="s">
         <v>92</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="D9" s="17" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="10" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="10" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="10" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1305,30 +1363,30 @@
         <v>34</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="E13" s="13" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="10" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1336,81 +1394,81 @@
         <v>50</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="E15" s="13" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="10" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="10" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="E17" s="13" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="10" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="10" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="D19" s="17" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="E19" s="13" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1418,51 +1476,51 @@
         <v>36</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="D20" s="17" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="E20" s="13" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="10" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="D21" s="17" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="10" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="B22" s="11"/>
       <c r="C22" s="10" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="D22" s="12"/>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="18" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="D23" s="12"/>
     </row>

</xml_diff>